<commit_message>
refactor: review 00-3f standard non-flag instructions
</commit_message>
<xml_diff>
--- a/docs/Z80.xlsx
+++ b/docs/Z80.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dotne\source\repos\kliveide\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{756094DE-C507-4DAF-9BC2-9F3F93C0A57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C654485E-11AC-42CF-A1DC-6C87C54F7685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{5CA8A63B-F490-42DA-8730-76D66EBE7502}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{5CA8A63B-F490-42DA-8730-76D66EBE7502}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard" sheetId="2" r:id="rId1"/>
@@ -3663,7 +3663,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3672,13 +3672,26 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3690,14 +3703,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Jelölőszín 1" xfId="1" builtinId="29"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="119">
@@ -4734,8 +4750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04B26D1-A31D-4795-A91D-A81DC5C601BD}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4852,16 +4868,16 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -4870,22 +4886,22 @@
       <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -4894,7 +4910,7 @@
       <c r="O3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -4905,16 +4921,16 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -4923,22 +4939,22 @@
       <c r="G4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>60</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -4947,7 +4963,7 @@
       <c r="O4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>63</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -4961,13 +4977,13 @@
       <c r="B5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -4976,7 +4992,7 @@
       <c r="G5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -4988,10 +5004,10 @@
       <c r="K5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -5000,7 +5016,7 @@
       <c r="O5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="2" t="s">
         <v>79</v>
       </c>
       <c r="Q5" s="1" t="s">
@@ -5014,13 +5030,13 @@
       <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -5029,7 +5045,7 @@
       <c r="G6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -5041,10 +5057,10 @@
       <c r="K6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="2" t="s">
         <v>92</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -5053,7 +5069,7 @@
       <c r="O6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Q6" s="1" t="s">
@@ -9330,7 +9346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC54877C-0099-46F6-90F7-92BA5AA488CC}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>